<commit_message>
final two papers for batch 2
</commit_message>
<xml_diff>
--- a/Randomisation/SecondSampleRanks.xlsx
+++ b/Randomisation/SecondSampleRanks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saoirsekelleher/Documents/Research/QAEco/DOM_Review/Randomisation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3B099A-7CCC-7C4F-ADEA-3BACEDB8A88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E783F8C7-5E71-D64B-9C1D-9DF92789128F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4518,8 +4518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A570" workbookViewId="0">
-      <selection activeCell="D575" sqref="D575"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9520,48 +9520,48 @@
       </c>
     </row>
     <row r="218" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A218" t="s">
-        <v>7</v>
-      </c>
-      <c r="B218">
+      <c r="A218" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B218" s="1">
         <v>1177</v>
       </c>
-      <c r="C218" s="2" t="s">
+      <c r="C218" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D218" t="s">
-        <v>219</v>
-      </c>
-      <c r="E218">
+      <c r="D218" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E218" s="1">
         <v>24</v>
       </c>
-      <c r="F218">
+      <c r="F218" s="1">
         <v>11</v>
       </c>
-      <c r="G218" t="s">
+      <c r="G218" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="219" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A219" t="s">
-        <v>7</v>
-      </c>
-      <c r="B219">
+      <c r="A219" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B219" s="4">
         <v>1123</v>
       </c>
-      <c r="C219" s="2" t="s">
+      <c r="C219" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="D219" t="s">
-        <v>219</v>
-      </c>
-      <c r="E219">
+      <c r="D219" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="E219" s="4">
         <v>29</v>
       </c>
-      <c r="F219">
+      <c r="F219" s="4">
         <v>12</v>
       </c>
-      <c r="G219" t="s">
+      <c r="G219" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -9842,25 +9842,25 @@
       </c>
     </row>
     <row r="232" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A232" t="s">
-        <v>7</v>
-      </c>
-      <c r="B232">
+      <c r="A232" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B232" s="8">
         <v>1091</v>
       </c>
-      <c r="C232" s="2" t="s">
+      <c r="C232" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="D232" t="s">
-        <v>219</v>
-      </c>
-      <c r="E232">
+      <c r="D232" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="E232" s="8">
         <v>70</v>
       </c>
-      <c r="F232">
+      <c r="F232" s="8">
         <v>25</v>
       </c>
-      <c r="G232" t="s">
+      <c r="G232" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -18236,7 +18236,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="597" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="597" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A597" t="s">
         <v>7</v>
       </c>
@@ -18420,7 +18420,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="605" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="605" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A605" t="s">
         <v>7</v>
       </c>
@@ -18788,7 +18788,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="621" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="621" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A621" t="s">
         <v>7</v>
       </c>
@@ -19478,7 +19478,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="651" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="651" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A651" t="s">
         <v>7</v>
       </c>
@@ -19869,7 +19869,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="668" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+    <row r="668" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A668" t="s">
         <v>7</v>
       </c>
@@ -20812,7 +20812,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="709" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="709" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A709" t="s">
         <v>7</v>
       </c>
@@ -21042,7 +21042,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="719" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="719" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A719" t="s">
         <v>7</v>
       </c>
@@ -21709,7 +21709,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="748" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="748" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A748" t="s">
         <v>7</v>
       </c>
@@ -21870,7 +21870,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="755" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="755" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A755" t="s">
         <v>7</v>
       </c>
@@ -22284,7 +22284,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="773" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="773" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A773" t="s">
         <v>7</v>
       </c>
@@ -22353,7 +22353,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="776" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="776" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A776" t="s">
         <v>7</v>
       </c>
@@ -22422,7 +22422,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="779" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="779" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A779" t="s">
         <v>7</v>
       </c>
@@ -22445,7 +22445,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="780" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="780" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A780" t="s">
         <v>7</v>
       </c>
@@ -22560,7 +22560,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="785" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="785" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A785" t="s">
         <v>7</v>
       </c>
@@ -22629,7 +22629,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="788" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="788" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A788" t="s">
         <v>7</v>
       </c>
@@ -22951,7 +22951,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="802" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="802" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A802" t="s">
         <v>7</v>
       </c>
@@ -23296,7 +23296,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="817" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="817" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A817" t="s">
         <v>7</v>
       </c>
@@ -24354,7 +24354,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="863" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+    <row r="863" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A863" t="s">
         <v>7</v>
       </c>
@@ -24400,7 +24400,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="865" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="865" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A865" t="s">
         <v>7</v>
       </c>
@@ -24492,7 +24492,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="869" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="869" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A869" t="s">
         <v>7</v>
       </c>
@@ -25228,7 +25228,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="901" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="901" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A901" t="s">
         <v>7</v>
       </c>
@@ -25688,7 +25688,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="921" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+    <row r="921" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A921" t="s">
         <v>7</v>
       </c>
@@ -25734,7 +25734,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="923" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+    <row r="923" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A923" t="s">
         <v>7</v>
       </c>
@@ -26079,7 +26079,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="938" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="938" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A938" t="s">
         <v>7</v>
       </c>
@@ -26792,7 +26792,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="969" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="969" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A969" t="s">
         <v>7</v>
       </c>
@@ -26930,7 +26930,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="975" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="975" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A975" t="s">
         <v>7</v>
       </c>
@@ -27206,7 +27206,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="987" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="987" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A987" t="s">
         <v>7</v>
       </c>
@@ -27298,7 +27298,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="991" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="991" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A991" t="s">
         <v>7</v>
       </c>
@@ -27321,7 +27321,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="992" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+    <row r="992" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A992" t="s">
         <v>7</v>
       </c>
@@ -29345,7 +29345,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="1080" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="1080" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A1080" t="s">
         <v>7</v>
       </c>
@@ -29621,7 +29621,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="1092" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="1092" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A1092" t="s">
         <v>7</v>
       </c>
@@ -29667,7 +29667,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="1094" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="1094" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A1094" t="s">
         <v>7</v>
       </c>
@@ -29828,7 +29828,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="1101" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+    <row r="1101" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A1101" t="s">
         <v>7</v>
       </c>
@@ -29989,7 +29989,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="1108" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="1108" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A1108" t="s">
         <v>7</v>
       </c>
@@ -30150,7 +30150,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="1115" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="1115" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A1115" t="s">
         <v>7</v>
       </c>
@@ -30334,7 +30334,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="1123" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="1123" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A1123" t="s">
         <v>7</v>
       </c>

</xml_diff>